<commit_message>
progress 5/6 remember to check one of the commented methods
</commit_message>
<xml_diff>
--- a/tracking_tables.xlsx
+++ b/tracking_tables.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itayk\Documents\dev\c#\Josef_Baron\program-design-h.w-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50AEA94-0EED-40C9-AB37-CAF458E4F310}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CE19F9-40A2-4F38-BB40-93D4E6B264EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="75">
   <si>
     <t>x</t>
   </si>
@@ -133,13 +134,139 @@
   </si>
   <si>
     <t>11 - is prime</t>
+  </si>
+  <si>
+    <t>que</t>
+  </si>
+  <si>
+    <t>[5,2,13,54]</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>que =       [ [5,2,13,54] , [] , [841,27,500] , [12] , [7,2,4,3,11] , [8,5] ]</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>head-----------------------------------------------------------------------tail</t>
+  </si>
+  <si>
+    <t>! q.isEmpty()</t>
+  </si>
+  <si>
+    <t>count != 0</t>
+  </si>
+  <si>
+    <t>return</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[] , [841,27,500] , [12] , [7,2,4,3,11] , [8,5] ]</t>
+  </si>
+  <si>
+    <t>[2,13,54]</t>
+  </si>
+  <si>
+    <t>[13,54]</t>
+  </si>
+  <si>
+    <t>[54]</t>
+  </si>
+  <si>
+    <t>qNew</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[841,27,500] , [12] , [7,2,4,3,11] , [8,5] ]</t>
+  </si>
+  <si>
+    <t>while status</t>
+  </si>
+  <si>
+    <t>begin{</t>
+  </si>
+  <si>
+    <t>}end</t>
+  </si>
+  <si>
+    <t>begin{}end</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[12] , [7,2,4,3,11] , [8,5] ]</t>
+  </si>
+  <si>
+    <t>[18.5]</t>
+  </si>
+  <si>
+    <t>[841,27,500]</t>
+  </si>
+  <si>
+    <t>[27,500]</t>
+  </si>
+  <si>
+    <t>[500]</t>
+  </si>
+  <si>
+    <t>[18.5,456]</t>
+  </si>
+  <si>
+    <t>[12]</t>
+  </si>
+  <si>
+    <t>[18.5,456,12]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[7,2,4,3,11] , [8,5] ]</t>
+  </si>
+  <si>
+    <t>[7,2,4,3,11]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[8,5] ]</t>
+  </si>
+  <si>
+    <t>[2,4,3,11]</t>
+  </si>
+  <si>
+    <t>[4,3,11]</t>
+  </si>
+  <si>
+    <t>[11]</t>
+  </si>
+  <si>
+    <t>[8,5]</t>
+  </si>
+  <si>
+    <t>[8]</t>
+  </si>
+  <si>
+    <t>[18.5,456,12,5.4,6.5]</t>
+  </si>
+  <si>
+    <t>[18.5,456,12,5.4]</t>
+  </si>
+  <si>
+    <t>טענת יציאה היא אם que ריק</t>
+  </si>
+  <si>
+    <t>מטרת הפעולה היא ליצור טור של כל הממוצעים של כל התואים המלאים בque</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,16 +280,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -170,17 +309,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="44">
@@ -648,15 +806,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3006845-BE2E-407E-80E5-C2D89E814DCE}" name="Table1" displayName="Table1" ref="W23:AC31" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3006845-BE2E-407E-80E5-C2D89E814DCE}" name="Table1" displayName="Table1" ref="W23:AC31" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="W23:AC31" xr:uid="{2DD0A4C5-FE0E-46B2-A46F-209E14B3D584}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BBC26616-07B1-4F89-836E-DE90DC98CC8D}" name="way in return " dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{A95CF8FA-116B-42BC-8D5C-2E9F840C2A7C}" name="way out return" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{7A3D3C2C-BF6B-4A8F-A31A-5443534D07E9}" name="x" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{D34B628F-6EFD-48DF-A704-C6301814E43C}" name="num" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{D8CB43B7-8F05-489E-95DE-929349D0DED9}" name="num %10== x" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{F7505246-5FD6-4722-A628-7D3EFFC93A49}" name="num == 0" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{BBC26616-07B1-4F89-836E-DE90DC98CC8D}" name="way in return " dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{A95CF8FA-116B-42BC-8D5C-2E9F840C2A7C}" name="way out return" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{7A3D3C2C-BF6B-4A8F-A31A-5443534D07E9}" name="x" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{D34B628F-6EFD-48DF-A704-C6301814E43C}" name="num" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{D8CB43B7-8F05-489E-95DE-929349D0DED9}" name="num %10== x" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{F7505246-5FD6-4722-A628-7D3EFFC93A49}" name="num == 0" dataDxfId="36"/>
     <tableColumn id="14" xr3:uid="{A1C468CF-44A2-490E-AB58-524D99142D38}" name="final - output" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -664,48 +822,48 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2538C69-7DA0-46DE-80FF-21BB3D373552}" name="Table2" displayName="Table2" ref="W33:AC45" totalsRowShown="0" headerRowDxfId="26" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2538C69-7DA0-46DE-80FF-21BB3D373552}" name="Table2" displayName="Table2" ref="W33:AC45" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="W33:AC45" xr:uid="{8BC88683-DB27-4003-AC36-DB5B0B7BED14}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F0003DB1-1D3F-4D29-B14C-5299BF5F8A43}" name="way in return " dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{D6AFACCB-5FFA-47FB-B8B3-723A9A8E5724}" name="way out return" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{18BF5EA2-7C4F-4D6D-A393-8C75C297A8B9}" name="a" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{FDDC3A04-9D7A-40D9-8DE2-061832C0FC20}" name="k" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{9ADF7E70-ED7F-4538-88BF-76C5B72F6D70}" name="k== a.length - 1" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{BD7C0992-8F68-4DBC-A2CF-BA7ABF692DF6}" name="FirstCheck(x, num / 10) " dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{3364A6E8-4967-41F4-B90A-6F4323EA117B}" name="final - output" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{F0003DB1-1D3F-4D29-B14C-5299BF5F8A43}" name="way in return " dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{D6AFACCB-5FFA-47FB-B8B3-723A9A8E5724}" name="way out return" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{18BF5EA2-7C4F-4D6D-A393-8C75C297A8B9}" name="a" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{FDDC3A04-9D7A-40D9-8DE2-061832C0FC20}" name="k" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{9ADF7E70-ED7F-4538-88BF-76C5B72F6D70}" name="k== a.length - 1" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{BD7C0992-8F68-4DBC-A2CF-BA7ABF692DF6}" name="FirstCheck(x, num / 10) " dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{3364A6E8-4967-41F4-B90A-6F4323EA117B}" name="final - output" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9BF24C51-FED9-4E38-ADF5-8E661701F830}" name="Table3" displayName="Table3" ref="N16:T22" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9BF24C51-FED9-4E38-ADF5-8E661701F830}" name="Table3" displayName="Table3" ref="N16:T22" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="N16:T22" xr:uid="{C74317DD-C71E-4A38-95BD-D76CCB7A557C}"/>
   <tableColumns count="7">
-    <tableColumn id="11" xr3:uid="{224729A1-A425-45DA-AC86-015AA03E6D95}" name="way in return " dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{75709B9F-3A1F-48F0-B5EC-5E1C879C22C0}" name="way out return" dataDxfId="24"/>
-    <tableColumn id="1" xr3:uid="{A68A2E43-8A30-41BD-AC2B-77E7BD20559B}" name="n" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{1BCAAF84-F0F0-410F-924A-D3BB77E99C9C}" name="k" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{0CE9F502-FA61-47E3-B926-41575FFF455D}" name="n&lt;k" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{B990108A-5F9A-442E-ACCC-B0F568F80E75}" name="n == k" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{ACADF1A2-58F3-436E-BC79-3723BE6E01CF}" name="final output" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{224729A1-A425-45DA-AC86-015AA03E6D95}" name="way in return " dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{75709B9F-3A1F-48F0-B5EC-5E1C879C22C0}" name="way out return" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{A68A2E43-8A30-41BD-AC2B-77E7BD20559B}" name="n" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{1BCAAF84-F0F0-410F-924A-D3BB77E99C9C}" name="k" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{0CE9F502-FA61-47E3-B926-41575FFF455D}" name="n&lt;k" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{B990108A-5F9A-442E-ACCC-B0F568F80E75}" name="n == k" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{ACADF1A2-58F3-436E-BC79-3723BE6E01CF}" name="final output" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A0B63A9F-E023-4A3F-B92B-E85C4580CB2C}" name="Table4" displayName="Table4" ref="N25:T35" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A0B63A9F-E023-4A3F-B92B-E85C4580CB2C}" name="Table4" displayName="Table4" ref="N25:T35" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="N25:T35" xr:uid="{649EA836-B158-4501-B9B7-7A083E744ACF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2F25F909-1893-454A-8351-6D88651B7E20}" name="way in return " dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{AC04ACCB-5B7F-4686-8DB7-1315E5C66C71}" name="way out return" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{C1310840-E364-484D-A35E-12B57D42F30B}" name="n" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{37E1B357-F03E-46CE-B08C-B9F9870F66FE}" name="k" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{26B622B7-E6DD-4675-9275-984E6A1990C7}" name="CheckDiv(n, k)" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{1F65596E-D8F6-43B3-B8CE-0CD52744DCB8}" name="k==1" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{6E83AF33-2EA9-4903-9951-26157DD7EFAD}" name="final output" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{2F25F909-1893-454A-8351-6D88651B7E20}" name="way in return " dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{AC04ACCB-5B7F-4686-8DB7-1315E5C66C71}" name="way out return" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{C1310840-E364-484D-A35E-12B57D42F30B}" name="n" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{37E1B357-F03E-46CE-B08C-B9F9870F66FE}" name="k" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{26B622B7-E6DD-4675-9275-984E6A1990C7}" name="CheckDiv(n, k)" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{1F65596E-D8F6-43B3-B8CE-0CD52744DCB8}" name="k==1" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{6E83AF33-2EA9-4903-9951-26157DD7EFAD}" name="final output" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -721,6 +879,24 @@
     <tableColumn id="4" xr3:uid="{1E3343C0-E197-4677-860A-AB52EEC39CA1}" name="n" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{8118E620-4F27-4D89-AACA-E0139106E1C8}" name="checkPrime(a[n],a[n-1])" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{B9ACBA1E-BA63-466D-9477-B2E73DAC4C6A}" name="output" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{BB01DEAC-6FDE-4011-A9FC-4AB020ACC2D4}" name="Table6" displayName="Table6" ref="C8:K29" totalsRowShown="0">
+  <autoFilter ref="C8:K29" xr:uid="{29C5FCF8-1622-45B2-B63B-608DB71D7C46}"/>
+  <tableColumns count="9">
+    <tableColumn id="12" xr3:uid="{40ECCEC9-9729-45FC-8229-A3D6DD4319B8}" name="while status"/>
+    <tableColumn id="1" xr3:uid="{280BCE6A-82AD-4068-BAC3-66A7D5FC8853}" name="que"/>
+    <tableColumn id="2" xr3:uid="{3727D287-B678-4EC5-89EE-4CFE0DEDDDEB}" name="q"/>
+    <tableColumn id="3" xr3:uid="{F21A2BB8-6AB1-4E2B-AEC3-08E2B67D8998}" name="sum"/>
+    <tableColumn id="4" xr3:uid="{B1759783-E2E1-4D38-B90A-1587B196AF6B}" name="count"/>
+    <tableColumn id="5" xr3:uid="{65D8BB89-90EB-42EB-966C-D780E9016C1A}" name="! q.isEmpty()"/>
+    <tableColumn id="6" xr3:uid="{C7708AD1-7F88-4AE7-A264-11E4FBB9D8EF}" name="count != 0"/>
+    <tableColumn id="9" xr3:uid="{706E81B3-135B-435E-98FB-BB866893FD23}" name="qNew"/>
+    <tableColumn id="7" xr3:uid="{926815C9-5555-4980-B3E3-A3B12C424253}" name="return"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1623,7 +1799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1092726-912B-4CD0-8E09-A0B8E890167F}">
   <dimension ref="N16:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="G34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="T48" sqref="T48"/>
     </sheetView>
   </sheetViews>
@@ -2538,4 +2714,694 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C117AC-A4C3-4AB2-B317-160FFA267934}">
+  <dimension ref="C3:K34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="14" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="3:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13">
+        <v>74</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16">
+        <v>841</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17">
+        <v>868</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18">
+        <v>1368</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20">
+        <v>12</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>62</v>
+      </c>
+      <c r="K20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" t="s">
+        <v>62</v>
+      </c>
+      <c r="K21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" t="s">
+        <v>62</v>
+      </c>
+      <c r="K23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24">
+        <v>13</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25">
+        <v>16</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" t="s">
+        <v>72</v>
+      </c>
+      <c r="K26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" t="s">
+        <v>72</v>
+      </c>
+      <c r="K27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28">
+        <v>13</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I29" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" t="s">
+        <v>71</v>
+      </c>
+      <c r="K29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
one last thing left
</commit_message>
<xml_diff>
--- a/tracking_tables.xlsx
+++ b/tracking_tables.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itayk\Documents\dev\c#\Josef_Baron\program-design-h.w-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CE19F9-40A2-4F38-BB40-93D4E6B264EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331B9426-E0E0-4FE5-95DE-6E6BE1C6F743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="88">
   <si>
     <t>x</t>
   </si>
@@ -260,6 +261,45 @@
   </si>
   <si>
     <t>מטרת הפעולה היא ליצור טור של כל הממוצעים של כל התואים המלאים בque</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Trouble(double a,double b)</t>
+  </si>
+  <si>
+    <t>Touble(5,5) = 5</t>
+  </si>
+  <si>
+    <t>Trouble(4,4) = 4</t>
+  </si>
+  <si>
+    <t>Touble(7,3) = 5</t>
+  </si>
+  <si>
+    <t>Trouble(5,4)  = 4.5</t>
+  </si>
+  <si>
+    <t>Trouble(1,4) = 4</t>
+  </si>
+  <si>
+    <t>Touble(2,5) = 4</t>
+  </si>
+  <si>
+    <t>Trouble(2,2) = 4</t>
+  </si>
+  <si>
+    <t>Trouble(4,2) = 3</t>
   </si>
 </sst>
 </file>
@@ -341,7 +381,49 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="58">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -806,79 +888,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3006845-BE2E-407E-80E5-C2D89E814DCE}" name="Table1" displayName="Table1" ref="W23:AC31" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C3006845-BE2E-407E-80E5-C2D89E814DCE}" name="Table1" displayName="Table1" ref="W23:AC31" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="W23:AC31" xr:uid="{2DD0A4C5-FE0E-46B2-A46F-209E14B3D584}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{BBC26616-07B1-4F89-836E-DE90DC98CC8D}" name="way in return " dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{A95CF8FA-116B-42BC-8D5C-2E9F840C2A7C}" name="way out return" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{7A3D3C2C-BF6B-4A8F-A31A-5443534D07E9}" name="x" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{D34B628F-6EFD-48DF-A704-C6301814E43C}" name="num" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{D8CB43B7-8F05-489E-95DE-929349D0DED9}" name="num %10== x" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{F7505246-5FD6-4722-A628-7D3EFFC93A49}" name="num == 0" dataDxfId="36"/>
-    <tableColumn id="14" xr3:uid="{A1C468CF-44A2-490E-AB58-524D99142D38}" name="final - output" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{BBC26616-07B1-4F89-836E-DE90DC98CC8D}" name="way in return " dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{A95CF8FA-116B-42BC-8D5C-2E9F840C2A7C}" name="way out return" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{7A3D3C2C-BF6B-4A8F-A31A-5443534D07E9}" name="x" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{D34B628F-6EFD-48DF-A704-C6301814E43C}" name="num" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{D8CB43B7-8F05-489E-95DE-929349D0DED9}" name="num %10== x" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{F7505246-5FD6-4722-A628-7D3EFFC93A49}" name="num == 0" dataDxfId="50"/>
+    <tableColumn id="14" xr3:uid="{A1C468CF-44A2-490E-AB58-524D99142D38}" name="final - output" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2538C69-7DA0-46DE-80FF-21BB3D373552}" name="Table2" displayName="Table2" ref="W33:AC45" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2538C69-7DA0-46DE-80FF-21BB3D373552}" name="Table2" displayName="Table2" ref="W33:AC45" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="W33:AC45" xr:uid="{8BC88683-DB27-4003-AC36-DB5B0B7BED14}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F0003DB1-1D3F-4D29-B14C-5299BF5F8A43}" name="way in return " dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{D6AFACCB-5FFA-47FB-B8B3-723A9A8E5724}" name="way out return" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{18BF5EA2-7C4F-4D6D-A393-8C75C297A8B9}" name="a" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{FDDC3A04-9D7A-40D9-8DE2-061832C0FC20}" name="k" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{9ADF7E70-ED7F-4538-88BF-76C5B72F6D70}" name="k== a.length - 1" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{BD7C0992-8F68-4DBC-A2CF-BA7ABF692DF6}" name="FirstCheck(x, num / 10) " dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{3364A6E8-4967-41F4-B90A-6F4323EA117B}" name="final - output" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{F0003DB1-1D3F-4D29-B14C-5299BF5F8A43}" name="way in return " dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{D6AFACCB-5FFA-47FB-B8B3-723A9A8E5724}" name="way out return" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{18BF5EA2-7C4F-4D6D-A393-8C75C297A8B9}" name="a" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{FDDC3A04-9D7A-40D9-8DE2-061832C0FC20}" name="k" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{9ADF7E70-ED7F-4538-88BF-76C5B72F6D70}" name="k== a.length - 1" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{BD7C0992-8F68-4DBC-A2CF-BA7ABF692DF6}" name="FirstCheck(x, num / 10) " dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{3364A6E8-4967-41F4-B90A-6F4323EA117B}" name="final - output" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9BF24C51-FED9-4E38-ADF5-8E661701F830}" name="Table3" displayName="Table3" ref="N16:T22" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9BF24C51-FED9-4E38-ADF5-8E661701F830}" name="Table3" displayName="Table3" ref="N16:T22" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="N16:T22" xr:uid="{C74317DD-C71E-4A38-95BD-D76CCB7A557C}"/>
   <tableColumns count="7">
-    <tableColumn id="11" xr3:uid="{224729A1-A425-45DA-AC86-015AA03E6D95}" name="way in return " dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{75709B9F-3A1F-48F0-B5EC-5E1C879C22C0}" name="way out return" dataDxfId="22"/>
-    <tableColumn id="1" xr3:uid="{A68A2E43-8A30-41BD-AC2B-77E7BD20559B}" name="n" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{1BCAAF84-F0F0-410F-924A-D3BB77E99C9C}" name="k" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{0CE9F502-FA61-47E3-B926-41575FFF455D}" name="n&lt;k" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{B990108A-5F9A-442E-ACCC-B0F568F80E75}" name="n == k" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{ACADF1A2-58F3-436E-BC79-3723BE6E01CF}" name="final output" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{224729A1-A425-45DA-AC86-015AA03E6D95}" name="way in return " dataDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{75709B9F-3A1F-48F0-B5EC-5E1C879C22C0}" name="way out return" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{A68A2E43-8A30-41BD-AC2B-77E7BD20559B}" name="n" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{1BCAAF84-F0F0-410F-924A-D3BB77E99C9C}" name="k" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{0CE9F502-FA61-47E3-B926-41575FFF455D}" name="n&lt;k" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{B990108A-5F9A-442E-ACCC-B0F568F80E75}" name="n == k" dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{ACADF1A2-58F3-436E-BC79-3723BE6E01CF}" name="final output" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A0B63A9F-E023-4A3F-B92B-E85C4580CB2C}" name="Table4" displayName="Table4" ref="N25:T35" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A0B63A9F-E023-4A3F-B92B-E85C4580CB2C}" name="Table4" displayName="Table4" ref="N25:T35" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="N25:T35" xr:uid="{649EA836-B158-4501-B9B7-7A083E744ACF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2F25F909-1893-454A-8351-6D88651B7E20}" name="way in return " dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{AC04ACCB-5B7F-4686-8DB7-1315E5C66C71}" name="way out return" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{C1310840-E364-484D-A35E-12B57D42F30B}" name="n" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{37E1B357-F03E-46CE-B08C-B9F9870F66FE}" name="k" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{26B622B7-E6DD-4675-9275-984E6A1990C7}" name="CheckDiv(n, k)" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{1F65596E-D8F6-43B3-B8CE-0CD52744DCB8}" name="k==1" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{6E83AF33-2EA9-4903-9951-26157DD7EFAD}" name="final output" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{2F25F909-1893-454A-8351-6D88651B7E20}" name="way in return " dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{AC04ACCB-5B7F-4686-8DB7-1315E5C66C71}" name="way out return" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{C1310840-E364-484D-A35E-12B57D42F30B}" name="n" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{37E1B357-F03E-46CE-B08C-B9F9870F66FE}" name="k" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{26B622B7-E6DD-4675-9275-984E6A1990C7}" name="CheckDiv(n, k)" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{1F65596E-D8F6-43B3-B8CE-0CD52744DCB8}" name="k==1" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{6E83AF33-2EA9-4903-9951-26157DD7EFAD}" name="final output" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7769908A-CD5B-4B7B-9A64-2954150DDD87}" name="Table46" displayName="Table46" ref="N37:S59" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7769908A-CD5B-4B7B-9A64-2954150DDD87}" name="Table46" displayName="Table46" ref="N37:S59" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="N37:S59" xr:uid="{3C309C2F-5B4F-4878-ADB2-2427CB4B7499}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9C32E65E-0132-4756-94AA-01C56A0F9C78}" name="way in return " dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{A723A41F-A1A7-48FF-ACFE-6A1752CA10BA}" name="way out return" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{4F5048BF-B7F4-47EF-82CE-9701E764E20B}" name="a[n]" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1E3343C0-E197-4677-860A-AB52EEC39CA1}" name="n" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{8118E620-4F27-4D89-AACA-E0139106E1C8}" name="checkPrime(a[n],a[n-1])" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{B9ACBA1E-BA63-466D-9477-B2E73DAC4C6A}" name="output" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9C32E65E-0132-4756-94AA-01C56A0F9C78}" name="way in return " dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{A723A41F-A1A7-48FF-ACFE-6A1752CA10BA}" name="way out return" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{4F5048BF-B7F4-47EF-82CE-9701E764E20B}" name="a[n]" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{1E3343C0-E197-4677-860A-AB52EEC39CA1}" name="n" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{8118E620-4F27-4D89-AACA-E0139106E1C8}" name="checkPrime(a[n],a[n-1])" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{B9ACBA1E-BA63-466D-9477-B2E73DAC4C6A}" name="output" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -897,6 +979,34 @@
     <tableColumn id="6" xr3:uid="{C7708AD1-7F88-4AE7-A264-11E4FBB9D8EF}" name="count != 0"/>
     <tableColumn id="9" xr3:uid="{706E81B3-135B-435E-98FB-BB866893FD23}" name="qNew"/>
     <tableColumn id="7" xr3:uid="{926815C9-5555-4980-B3E3-A3B12C424253}" name="return"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{883871A9-C35C-4FFE-B778-BDFCA231A821}" name="Table7" displayName="Table7" ref="C4:G6" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="C4:G6" xr:uid="{6BA2D4F5-E9D1-4B33-A6AE-C9135DF9965E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{8B0BED84-AD13-4A68-BB81-527A971CB6BF}" name="t1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{BA08C68B-4871-40C2-9BB5-2AC159B928DF}" name="t2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{70C40710-63A1-4E4D-99ED-B3C738D6B54E}" name="a" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{64337FD1-DCDE-45CF-9724-9437FCF14F3E}" name="b" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{DF980D19-E637-40AA-8308-EA983E7FAB6F}" name="Trouble(double a,double b)" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D2157B8E-EEA4-4C33-B2EF-9AB4493F665A}" name="Table79" displayName="Table79" ref="C10:G16" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="C10:G16" xr:uid="{479E7F4B-5FDC-4F73-8A71-EB30F7673D97}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{4A5DA8AD-0808-412D-9DC7-60902873883E}" name="t1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{FD1A195A-A68D-4659-A62A-BA955088E688}" name="t2" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{634BC92B-B2EB-4017-812C-298EF548AC10}" name="a" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{2B0E9A79-500D-4E7D-AC82-0418F354A1ED}" name="b" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{C1A73EEB-18D1-44C9-939A-175A9C3751AC}" name="Trouble(double a,double b)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2720,7 +2830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C117AC-A4C3-4AB2-B317-160FFA267934}">
   <dimension ref="C3:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
@@ -3404,4 +3514,201 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23821811-D1CA-4B1B-A46E-E6DE4326BA50}">
+  <dimension ref="C4:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>